<commit_message>
almost done no more new files
there is just a little bit of modifications needed and i wont add new files it will be only on this file (semi = semi final)
</commit_message>
<xml_diff>
--- a/test_1.xlsx
+++ b/test_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="checkout" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -54,9 +56,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,32 +410,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="14.109375" customWidth="1" min="1" max="1"/>
     <col width="11.6640625" customWidth="1" min="2" max="2"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Table Number</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Orders</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -437,16 +433,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="16.6640625" customWidth="1" min="1" max="1"/>
-    <col width="16.44140625" customWidth="1" min="2" max="2"/>
+    <col width="18.109375" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="11.33203125" customWidth="1" min="3" max="3"/>
     <col width="10" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="8.77734375" bestFit="1" customWidth="1" min="5" max="5"/>
@@ -455,123 +451,124 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>table num</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>orders</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
+          <t>table Number</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Orders</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>09/07/2023 20:02:15</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ice tea</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>09/07/2023 20:02:23</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ice cream</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09/07/2023 20:03:58</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ice 3 in 1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ice coffee</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>09/07/2023 20:24:16</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>tea</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>09/07/2023 20:24:22</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>coffee</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>tea</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ice tea</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>09/07/2023 20:24:33</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>3 in 1</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>tea</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>coffee</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>tea</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hot coffee</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ice coffee</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>ice 3 in 1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>3 in 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>spaghetti</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>lettuce</t>
         </is>
       </c>
     </row>

</xml_diff>